<commit_message>
fixes documentation handling for topiclinks, fixes tests and regenerates examples
</commit_message>
<xml_diff>
--- a/examples/ceur-ws/ceur-ws.xlsx
+++ b/examples/ceur-ws/ceur-ws.xlsx
@@ -415,7 +415,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D1"/>
+  <dimension ref="A1:F1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -442,6 +442,16 @@
       <c r="D1" t="inlineStr">
         <is>
           <t>paper__pdfUrl</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>paper__volume</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>paper__session</t>
         </is>
       </c>
     </row>
@@ -456,7 +466,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:A1"/>
+  <dimension ref="A1:B1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -468,6 +478,11 @@
       <c r="A1" t="inlineStr">
         <is>
           <t>session__title</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>session__volume</t>
         </is>
       </c>
     </row>

</xml_diff>